<commit_message>
Ajout des URLs directes
</commit_message>
<xml_diff>
--- a/RiC-O_0-2_listOfClasses.xlsx
+++ b/RiC-O_0-2_listOfClasses.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="349">
   <si>
     <t xml:space="preserve">Ontology IRI</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lien direct vers le fichier RDF :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://xls2rdf.sparna.fr/rest/convert?url=https%3A%2F%2Fgithub.com%2Fsparna-git%2Fsparnatural-demonstrateur-an%2Fraw%2Fmain%2FRiC-O_0-2_listOfClasses.xlsx&amp;noPostProcessings=true</t>
   </si>
   <si>
     <t xml:space="preserve">identifiant dans l’IRI</t>
@@ -1204,7 +1207,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1227,6 +1230,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1353,8 +1360,8 @@
   </sheetPr>
   <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1406,7 +1413,7 @@
       <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2"/>
@@ -1415,10 +1422,12 @@
       <c r="E5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1429,36 +1438,36 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" s="10" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="8" t="s">
+    <row r="8" s="11" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" s="10" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="12" t="s">
+    </row>
+    <row r="9" s="11" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="B9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>12</v>
+      <c r="C9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1466,15 +1475,15 @@
         <f aca="false">CONCATENATE($B$2,":",B10)</f>
         <v>rico:AccumulationRelation</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16" t="s">
+      <c r="C10" s="16" t="s">
         <v>16</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,17 +1491,17 @@
         <f aca="false">CONCATENATE($B$2,":",B11)</f>
         <v>rico:Activity</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="B11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="C11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>19</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,17 +1509,17 @@
         <f aca="false">CONCATENATE($B$2,":",B12)</f>
         <v>rico:ActivityDocumentationRelation</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="C12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>23</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,17 +1527,17 @@
         <f aca="false">CONCATENATE($B$2,":",B13)</f>
         <v>rico:ActivityType</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>27</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,17 +1545,17 @@
         <f aca="false">CONCATENATE($B$2,":",B14)</f>
         <v>rico:Agent</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="16" t="s">
+      <c r="B14" s="16" t="s">
         <v>29</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,15 +1563,15 @@
         <f aca="false">CONCATENATE($B$2,":",B15)</f>
         <v>rico:AgentControlRelation</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>32</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,15 +1579,15 @@
         <f aca="false">CONCATENATE($B$2,":",B16)</f>
         <v>rico:AgentHierarchicalRelation</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="15" t="s">
+      <c r="B16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>35</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,17 +1595,17 @@
         <f aca="false">CONCATENATE($B$2,":",B17)</f>
         <v>rico:AgentName</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="15" t="s">
+      <c r="B17" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="C17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="D17" s="16" t="s">
         <v>39</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,17 +1613,17 @@
         <f aca="false">CONCATENATE($B$2,":",B18)</f>
         <v>rico:AgentOriginationRelation</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="C18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>43</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,15 +1631,15 @@
         <f aca="false">CONCATENATE($B$2,":",B19)</f>
         <v>rico:AgentTemporalRelation</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="15" t="s">
+      <c r="B19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>46</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,15 +1647,15 @@
         <f aca="false">CONCATENATE($B$2,":",B20)</f>
         <v>rico:AgentToAgentRelation</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16" t="s">
+      <c r="C20" s="16" t="s">
         <v>49</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,17 +1663,17 @@
         <f aca="false">CONCATENATE($B$2,":",B21)</f>
         <v>rico:Appellation</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="16" t="s">
+      <c r="B21" s="16" t="s">
         <v>51</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,15 +1681,15 @@
         <f aca="false">CONCATENATE($B$2,":",B22)</f>
         <v>rico:AppellationRelation</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16" t="s">
+      <c r="C22" s="16" t="s">
         <v>54</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,15 +1697,15 @@
         <f aca="false">CONCATENATE($B$2,":",B23)</f>
         <v>rico:AuthorityRelation</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16" t="s">
+      <c r="C23" s="16" t="s">
         <v>57</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1704,15 +1713,15 @@
         <f aca="false">CONCATENATE($B$2,":",B24)</f>
         <v>rico:AuthorshipRelation</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="15" t="s">
+      <c r="B24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>60</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,15 +1729,15 @@
         <f aca="false">CONCATENATE($B$2,":",B25)</f>
         <v>rico:CarrierExtent</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="15" t="s">
+      <c r="B25" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16" t="s">
+      <c r="C25" s="16" t="s">
         <v>63</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,17 +1745,17 @@
         <f aca="false">CONCATENATE($B$2,":",B26)</f>
         <v>rico:CarrierType</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="C26" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="D26" s="16" t="s">
         <v>67</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1754,15 +1763,15 @@
         <f aca="false">CONCATENATE($B$2,":",B27)</f>
         <v>rico:ChildRelation</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>70</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,17 +1779,17 @@
         <f aca="false">CONCATENATE($B$2,":",B28)</f>
         <v>rico:Concept</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="16" t="s">
+      <c r="B28" s="16" t="s">
         <v>72</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,15 +1797,15 @@
         <f aca="false">CONCATENATE($B$2,":",B29)</f>
         <v>rico:ContentType</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16" t="s">
+      <c r="C29" s="16" t="s">
         <v>75</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,17 +1813,17 @@
         <f aca="false">CONCATENATE($B$2,":",B30)</f>
         <v>rico:Coordinates</v>
       </c>
-      <c r="B30" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="15" t="s">
+      <c r="B30" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="C30" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="16" t="s">
         <v>78</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,17 +1831,17 @@
         <f aca="false">CONCATENATE($B$2,":",B31)</f>
         <v>rico:CorporateBody</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="15" t="s">
+      <c r="B31" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="C31" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="D31" s="16" t="s">
         <v>82</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,17 +1849,17 @@
         <f aca="false">CONCATENATE($B$2,":",B32)</f>
         <v>rico:CorporateBodyType</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="15" t="s">
+      <c r="B32" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="C32" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="D32" s="16" t="s">
         <v>86</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,15 +1867,15 @@
         <f aca="false">CONCATENATE($B$2,":",B33)</f>
         <v>rico:CorrespondenceRelation</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="B33" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16" t="s">
+      <c r="C33" s="16" t="s">
         <v>89</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,15 +1883,15 @@
         <f aca="false">CONCATENATE($B$2,":",B34)</f>
         <v>rico:CreationRelation</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="16" t="s">
+      <c r="C34" s="16" t="s">
         <v>92</v>
+      </c>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,17 +1899,17 @@
         <f aca="false">CONCATENATE($B$2,":",B35)</f>
         <v>rico:Date</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="16" t="s">
+      <c r="B35" s="16" t="s">
         <v>94</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,15 +1917,15 @@
         <f aca="false">CONCATENATE($B$2,":",B36)</f>
         <v>rico:DateRange</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="15" t="s">
+      <c r="B36" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16" t="s">
+      <c r="C36" s="16" t="s">
         <v>97</v>
+      </c>
+      <c r="D36" s="16"/>
+      <c r="E36" s="17" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,15 +1933,15 @@
         <f aca="false">CONCATENATE($B$2,":",B37)</f>
         <v>rico:DateSet</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="15" t="s">
+      <c r="B37" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16" t="s">
+      <c r="C37" s="16" t="s">
         <v>100</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,15 +1949,15 @@
         <f aca="false">CONCATENATE($B$2,":",B38)</f>
         <v>rico:DemographicGroup</v>
       </c>
-      <c r="B38" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="15" t="s">
+      <c r="B38" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="16" t="s">
+      <c r="C38" s="16" t="s">
         <v>103</v>
+      </c>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,15 +1965,15 @@
         <f aca="false">CONCATENATE($B$2,":",B39)</f>
         <v>rico:DerivationRelation</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="15" t="s">
+      <c r="B39" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="16" t="s">
+      <c r="C39" s="16" t="s">
         <v>106</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="E39" s="17" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,15 +1981,15 @@
         <f aca="false">CONCATENATE($B$2,":",B40)</f>
         <v>rico:DescendanceRelation</v>
       </c>
-      <c r="B40" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="15" t="s">
+      <c r="B40" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="16" t="s">
+      <c r="C40" s="16" t="s">
         <v>109</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1988,17 +1997,17 @@
         <f aca="false">CONCATENATE($B$2,":",B41)</f>
         <v>rico:DocumentaryFormType</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" s="15" t="s">
+      <c r="B41" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="C41" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="D41" s="16" t="s">
         <v>113</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,17 +2015,17 @@
         <f aca="false">CONCATENATE($B$2,":",B42)</f>
         <v>rico:Event</v>
       </c>
-      <c r="B42" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="15" t="s">
+      <c r="B42" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="C42" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="16" t="s">
         <v>116</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,15 +2033,15 @@
         <f aca="false">CONCATENATE($B$2,":",B43)</f>
         <v>rico:EventRelation</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C43" s="15" t="s">
+      <c r="B43" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="16" t="s">
+      <c r="C43" s="16" t="s">
         <v>119</v>
+      </c>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2040,17 +2049,17 @@
         <f aca="false">CONCATENATE($B$2,":",B44)</f>
         <v>rico:EventType</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44" s="15" t="s">
+      <c r="B44" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="D44" s="16" t="s">
         <v>123</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,15 +2067,15 @@
         <f aca="false">CONCATENATE($B$2,":",B45)</f>
         <v>rico:Extent</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="16" t="s">
+      <c r="B45" s="16" t="s">
         <v>125</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="17" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2074,15 +2083,15 @@
         <f aca="false">CONCATENATE($B$2,":",B46)</f>
         <v>rico:ExtentType</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="15" t="s">
+      <c r="B46" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="16" t="s">
+      <c r="C46" s="16" t="s">
         <v>128</v>
+      </c>
+      <c r="D46" s="16"/>
+      <c r="E46" s="17" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,17 +2099,17 @@
         <f aca="false">CONCATENATE($B$2,":",B47)</f>
         <v>rico:Family</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D47" s="15" t="s">
+      <c r="B47" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="C47" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="16" t="s">
         <v>131</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,17 +2117,17 @@
         <f aca="false">CONCATENATE($B$2,":",B48)</f>
         <v>rico:FamilyRelation</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="15" t="s">
+      <c r="B48" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="C48" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="D48" s="16" t="s">
         <v>135</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2126,17 +2135,17 @@
         <f aca="false">CONCATENATE($B$2,":",B49)</f>
         <v>rico:FamilyType</v>
       </c>
-      <c r="B49" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" s="15" t="s">
+      <c r="B49" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="C49" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="D49" s="16" t="s">
         <v>139</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,15 +2153,15 @@
         <f aca="false">CONCATENATE($B$2,":",B50)</f>
         <v>rico:FunctionalEquivalenceRelation</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C50" s="15" t="s">
+      <c r="B50" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="D50" s="15"/>
-      <c r="E50" s="16" t="s">
+      <c r="C50" s="16" t="s">
         <v>142</v>
+      </c>
+      <c r="D50" s="16"/>
+      <c r="E50" s="17" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,17 +2169,17 @@
         <f aca="false">CONCATENATE($B$2,":",B51)</f>
         <v>rico:Group</v>
       </c>
-      <c r="B51" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D51" s="15" t="s">
+      <c r="B51" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="C51" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="16" t="s">
         <v>145</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,15 +2187,15 @@
         <f aca="false">CONCATENATE($B$2,":",B52)</f>
         <v>rico:GroupSubdivisionRelation</v>
       </c>
-      <c r="B52" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="15" t="s">
+      <c r="B52" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="16" t="s">
+      <c r="C52" s="16" t="s">
         <v>148</v>
+      </c>
+      <c r="D52" s="16"/>
+      <c r="E52" s="17" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,17 +2203,17 @@
         <f aca="false">CONCATENATE($B$2,":",B53)</f>
         <v>rico:Identifier</v>
       </c>
-      <c r="B53" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D53" s="15" t="s">
+      <c r="B53" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="C53" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" s="16" t="s">
         <v>151</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,17 +2221,17 @@
         <f aca="false">CONCATENATE($B$2,":",B54)</f>
         <v>rico:IdentifierType</v>
       </c>
-      <c r="B54" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" s="15" t="s">
+      <c r="B54" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="C54" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="D54" s="16" t="s">
         <v>155</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2230,17 +2239,17 @@
         <f aca="false">CONCATENATE($B$2,":",B55)</f>
         <v>rico:Instantiation</v>
       </c>
-      <c r="B55" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E55" s="16" t="s">
+      <c r="B55" s="16" t="s">
         <v>157</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2248,15 +2257,15 @@
         <f aca="false">CONCATENATE($B$2,":",B56)</f>
         <v>rico:InstantiationExtent</v>
       </c>
-      <c r="B56" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="C56" s="15" t="s">
+      <c r="B56" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="D56" s="15"/>
-      <c r="E56" s="16" t="s">
+      <c r="C56" s="16" t="s">
         <v>160</v>
+      </c>
+      <c r="D56" s="16"/>
+      <c r="E56" s="17" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,15 +2273,15 @@
         <f aca="false">CONCATENATE($B$2,":",B57)</f>
         <v>rico:InstantiationToInstantiationRelation</v>
       </c>
-      <c r="B57" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C57" s="15" t="s">
+      <c r="B57" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="D57" s="15"/>
-      <c r="E57" s="16" t="s">
+      <c r="C57" s="16" t="s">
         <v>163</v>
+      </c>
+      <c r="D57" s="16"/>
+      <c r="E57" s="17" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,15 +2289,15 @@
         <f aca="false">CONCATENATE($B$2,":",B58)</f>
         <v>rico:IntellectualPropertyRightsRelation</v>
       </c>
-      <c r="B58" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C58" s="15" t="s">
+      <c r="B58" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="16" t="s">
+      <c r="C58" s="16" t="s">
         <v>166</v>
+      </c>
+      <c r="D58" s="16"/>
+      <c r="E58" s="17" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,15 +2305,15 @@
         <f aca="false">CONCATENATE($B$2,":",B59)</f>
         <v>rico:KnowingOfRelation</v>
       </c>
-      <c r="B59" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C59" s="15" t="s">
+      <c r="B59" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="D59" s="15"/>
-      <c r="E59" s="16" t="s">
+      <c r="C59" s="16" t="s">
         <v>169</v>
+      </c>
+      <c r="D59" s="16"/>
+      <c r="E59" s="17" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,15 +2321,15 @@
         <f aca="false">CONCATENATE($B$2,":",B60)</f>
         <v>rico:KnowingRelation</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C60" s="15" t="s">
+      <c r="B60" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="D60" s="15"/>
-      <c r="E60" s="16" t="s">
+      <c r="C60" s="16" t="s">
         <v>172</v>
+      </c>
+      <c r="D60" s="16"/>
+      <c r="E60" s="17" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,17 +2337,17 @@
         <f aca="false">CONCATENATE($B$2,":",B61)</f>
         <v>rico:Language</v>
       </c>
-      <c r="B61" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" s="15" t="s">
+      <c r="B61" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="C61" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D61" s="16" t="s">
         <v>175</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,15 +2355,15 @@
         <f aca="false">CONCATENATE($B$2,":",B62)</f>
         <v>rico:LeadershipRelation</v>
       </c>
-      <c r="B62" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C62" s="15" t="s">
+      <c r="B62" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="D62" s="15"/>
-      <c r="E62" s="16" t="s">
+      <c r="C62" s="16" t="s">
         <v>178</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="17" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,17 +2371,17 @@
         <f aca="false">CONCATENATE($B$2,":",B63)</f>
         <v>rico:LegalStatus</v>
       </c>
-      <c r="B63" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C63" s="15" t="s">
+      <c r="B63" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="C63" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="D63" s="16" t="s">
         <v>182</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2380,15 +2389,15 @@
         <f aca="false">CONCATENATE($B$2,":",B64)</f>
         <v>rico:ManagementRelation</v>
       </c>
-      <c r="B64" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="C64" s="15" t="s">
+      <c r="B64" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="D64" s="15"/>
-      <c r="E64" s="16" t="s">
+      <c r="C64" s="16" t="s">
         <v>185</v>
+      </c>
+      <c r="D64" s="16"/>
+      <c r="E64" s="17" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,17 +2405,17 @@
         <f aca="false">CONCATENATE($B$2,":",B65)</f>
         <v>rico:Mandate</v>
       </c>
-      <c r="B65" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D65" s="15" t="s">
+      <c r="B65" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="C65" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="D65" s="16" t="s">
         <v>188</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2414,15 +2423,15 @@
         <f aca="false">CONCATENATE($B$2,":",B66)</f>
         <v>rico:MandateRelation</v>
       </c>
-      <c r="B66" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C66" s="15" t="s">
+      <c r="B66" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D66" s="15"/>
-      <c r="E66" s="16" t="s">
+      <c r="C66" s="16" t="s">
         <v>191</v>
+      </c>
+      <c r="D66" s="16"/>
+      <c r="E66" s="17" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,15 +2439,15 @@
         <f aca="false">CONCATENATE($B$2,":",B67)</f>
         <v>rico:Mechanism</v>
       </c>
-      <c r="B67" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="D67" s="15"/>
-      <c r="E67" s="16" t="s">
+      <c r="B67" s="16" t="s">
         <v>193</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D67" s="16"/>
+      <c r="E67" s="17" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,15 +2455,15 @@
         <f aca="false">CONCATENATE($B$2,":",B68)</f>
         <v>rico:MembershipRelation</v>
       </c>
-      <c r="B68" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="C68" s="15" t="s">
+      <c r="B68" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="D68" s="15"/>
-      <c r="E68" s="16" t="s">
+      <c r="C68" s="16" t="s">
         <v>196</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="17" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,15 +2471,15 @@
         <f aca="false">CONCATENATE($B$2,":",B69)</f>
         <v>rico:MigrationRelation</v>
       </c>
-      <c r="B69" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="C69" s="15" t="s">
+      <c r="B69" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="D69" s="15"/>
-      <c r="E69" s="16" t="s">
+      <c r="C69" s="16" t="s">
         <v>199</v>
+      </c>
+      <c r="D69" s="16"/>
+      <c r="E69" s="17" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,17 +2487,17 @@
         <f aca="false">CONCATENATE($B$2,":",B70)</f>
         <v>rico:Name</v>
       </c>
-      <c r="B70" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="D70" s="15" t="s">
+      <c r="B70" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="C70" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="D70" s="16" t="s">
         <v>202</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,17 +2505,17 @@
         <f aca="false">CONCATENATE($B$2,":",B71)</f>
         <v>rico:OccupationType</v>
       </c>
-      <c r="B71" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="C71" s="15" t="s">
+      <c r="B71" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="C71" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="D71" s="16" t="s">
         <v>206</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,15 +2523,15 @@
         <f aca="false">CONCATENATE($B$2,":",B72)</f>
         <v>rico:OwnershipRelation</v>
       </c>
-      <c r="B72" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="C72" s="15" t="s">
+      <c r="B72" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="D72" s="15"/>
-      <c r="E72" s="16" t="s">
+      <c r="C72" s="16" t="s">
         <v>209</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="17" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2530,15 +2539,15 @@
         <f aca="false">CONCATENATE($B$2,":",B73)</f>
         <v>rico:PerformanceRelation</v>
       </c>
-      <c r="B73" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="C73" s="15" t="s">
+      <c r="B73" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="D73" s="15"/>
-      <c r="E73" s="16" t="s">
+      <c r="C73" s="16" t="s">
         <v>212</v>
+      </c>
+      <c r="D73" s="16"/>
+      <c r="E73" s="17" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,17 +2555,17 @@
         <f aca="false">CONCATENATE($B$2,":",B74)</f>
         <v>rico:Person</v>
       </c>
-      <c r="B74" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D74" s="15" t="s">
+      <c r="B74" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="C74" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="D74" s="16" t="s">
         <v>215</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2564,15 +2573,15 @@
         <f aca="false">CONCATENATE($B$2,":",B75)</f>
         <v>rico:PhysicalLocation</v>
       </c>
-      <c r="B75" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="C75" s="15" t="s">
+      <c r="B75" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="D75" s="15"/>
-      <c r="E75" s="16" t="s">
+      <c r="C75" s="16" t="s">
         <v>218</v>
+      </c>
+      <c r="D75" s="16"/>
+      <c r="E75" s="17" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,17 +2589,17 @@
         <f aca="false">CONCATENATE($B$2,":",B76)</f>
         <v>rico:Place</v>
       </c>
-      <c r="B76" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D76" s="15" t="s">
+      <c r="B76" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="E76" s="16" t="s">
+      <c r="C76" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D76" s="16" t="s">
         <v>221</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,17 +2607,17 @@
         <f aca="false">CONCATENATE($B$2,":",B77)</f>
         <v>rico:PlaceName</v>
       </c>
-      <c r="B77" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="C77" s="15" t="s">
+      <c r="B77" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="D77" s="15" t="s">
+      <c r="C77" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="D77" s="16" t="s">
         <v>225</v>
+      </c>
+      <c r="E77" s="17" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,15 +2625,15 @@
         <f aca="false">CONCATENATE($B$2,":",B78)</f>
         <v>rico:PlaceRelation</v>
       </c>
-      <c r="B78" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="C78" s="15" t="s">
+      <c r="B78" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="D78" s="15"/>
-      <c r="E78" s="16" t="s">
+      <c r="C78" s="16" t="s">
         <v>228</v>
+      </c>
+      <c r="D78" s="16"/>
+      <c r="E78" s="17" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2632,17 +2641,17 @@
         <f aca="false">CONCATENATE($B$2,":",B79)</f>
         <v>rico:PlaceType</v>
       </c>
-      <c r="B79" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="C79" s="15" t="s">
+      <c r="B79" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="C79" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="D79" s="16" t="s">
         <v>232</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,17 +2659,17 @@
         <f aca="false">CONCATENATE($B$2,":",B80)</f>
         <v>rico:Position</v>
       </c>
-      <c r="B80" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="D80" s="15" t="s">
+      <c r="B80" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E80" s="16" t="s">
+      <c r="C80" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="16" t="s">
         <v>235</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2668,15 +2677,15 @@
         <f aca="false">CONCATENATE($B$2,":",B81)</f>
         <v>rico:PositionHoldingRelation</v>
       </c>
-      <c r="B81" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="C81" s="15" t="s">
+      <c r="B81" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="D81" s="15"/>
-      <c r="E81" s="16" t="s">
+      <c r="C81" s="16" t="s">
         <v>238</v>
+      </c>
+      <c r="D81" s="16"/>
+      <c r="E81" s="17" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,15 +2693,15 @@
         <f aca="false">CONCATENATE($B$2,":",B82)</f>
         <v>rico:PositionToGroupRelation</v>
       </c>
-      <c r="B82" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="C82" s="15" t="s">
+      <c r="B82" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="D82" s="15"/>
-      <c r="E82" s="16" t="s">
+      <c r="C82" s="16" t="s">
         <v>241</v>
+      </c>
+      <c r="D82" s="16"/>
+      <c r="E82" s="17" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,17 +2709,17 @@
         <f aca="false">CONCATENATE($B$2,":",B83)</f>
         <v>rico:ProductionTechniqueType</v>
       </c>
-      <c r="B83" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="C83" s="15" t="s">
+      <c r="B83" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="C83" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="D83" s="16" t="s">
         <v>245</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2718,17 +2727,17 @@
         <f aca="false">CONCATENATE($B$2,":",B84)</f>
         <v>rico:ProvenanceRelation</v>
       </c>
-      <c r="B84" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="C84" s="15" t="s">
+      <c r="B84" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="D84" s="15" t="s">
+      <c r="C84" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="D84" s="16" t="s">
         <v>249</v>
+      </c>
+      <c r="E84" s="17" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,15 +2745,15 @@
         <f aca="false">CONCATENATE($B$2,":",B85)</f>
         <v>rico:Proxy</v>
       </c>
-      <c r="B85" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="D85" s="15"/>
-      <c r="E85" s="16" t="s">
+      <c r="B85" s="16" t="s">
         <v>251</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D85" s="16"/>
+      <c r="E85" s="17" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,17 +2761,17 @@
         <f aca="false">CONCATENATE($B$2,":",B86)</f>
         <v>rico:Record</v>
       </c>
-      <c r="B86" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="D86" s="15" t="s">
+      <c r="B86" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="E86" s="16" t="s">
+      <c r="C86" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="D86" s="16" t="s">
         <v>254</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,17 +2779,17 @@
         <f aca="false">CONCATENATE($B$2,":",B87)</f>
         <v>rico:RecordPart</v>
       </c>
-      <c r="B87" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="C87" s="15" t="s">
+      <c r="B87" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="C87" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="E87" s="16" t="s">
+      <c r="D87" s="16" t="s">
         <v>258</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,17 +2797,17 @@
         <f aca="false">CONCATENATE($B$2,":",B88)</f>
         <v>rico:RecordResource</v>
       </c>
-      <c r="B88" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="C88" s="15" t="s">
+      <c r="B88" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="D88" s="15" t="s">
+      <c r="C88" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="E88" s="16" t="s">
+      <c r="D88" s="16" t="s">
         <v>262</v>
+      </c>
+      <c r="E88" s="17" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2806,15 +2815,15 @@
         <f aca="false">CONCATENATE($B$2,":",B89)</f>
         <v>rico:RecordResourceExtent</v>
       </c>
-      <c r="B89" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="C89" s="15" t="s">
+      <c r="B89" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="D89" s="15"/>
-      <c r="E89" s="16" t="s">
+      <c r="C89" s="16" t="s">
         <v>265</v>
+      </c>
+      <c r="D89" s="16"/>
+      <c r="E89" s="17" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2822,15 +2831,15 @@
         <f aca="false">CONCATENATE($B$2,":",B90)</f>
         <v>rico:RecordResourceGeneticRelation</v>
       </c>
-      <c r="B90" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="C90" s="15" t="s">
+      <c r="B90" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="D90" s="15"/>
-      <c r="E90" s="16" t="s">
+      <c r="C90" s="16" t="s">
         <v>268</v>
+      </c>
+      <c r="D90" s="16"/>
+      <c r="E90" s="17" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2838,15 +2847,15 @@
         <f aca="false">CONCATENATE($B$2,":",B91)</f>
         <v>rico:RecordResourceHoldingRelation</v>
       </c>
-      <c r="B91" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="C91" s="15" t="s">
+      <c r="B91" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="D91" s="15"/>
-      <c r="E91" s="16" t="s">
+      <c r="C91" s="16" t="s">
         <v>271</v>
+      </c>
+      <c r="D91" s="16"/>
+      <c r="E91" s="17" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,15 +2863,15 @@
         <f aca="false">CONCATENATE($B$2,":",B92)</f>
         <v>rico:RecordResourceToInstantiationRelation</v>
       </c>
-      <c r="B92" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="C92" s="15" t="s">
+      <c r="B92" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="D92" s="15"/>
-      <c r="E92" s="16" t="s">
+      <c r="C92" s="16" t="s">
         <v>274</v>
+      </c>
+      <c r="D92" s="16"/>
+      <c r="E92" s="17" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2870,15 +2879,15 @@
         <f aca="false">CONCATENATE($B$2,":",B93)</f>
         <v>rico:RecordResourceToRecordResourceRelation</v>
       </c>
-      <c r="B93" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="C93" s="15" t="s">
+      <c r="B93" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="D93" s="15"/>
-      <c r="E93" s="16" t="s">
+      <c r="C93" s="16" t="s">
         <v>277</v>
+      </c>
+      <c r="D93" s="16"/>
+      <c r="E93" s="17" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2886,17 +2895,17 @@
         <f aca="false">CONCATENATE($B$2,":",B94)</f>
         <v>rico:RecordSet</v>
       </c>
-      <c r="B94" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="C94" s="15" t="s">
+      <c r="B94" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="D94" s="15" t="s">
+      <c r="C94" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="D94" s="16" t="s">
         <v>281</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2904,17 +2913,17 @@
         <f aca="false">CONCATENATE($B$2,":",B95)</f>
         <v>rico:RecordSetType</v>
       </c>
-      <c r="B95" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="C95" s="15" t="s">
+      <c r="B95" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="D95" s="15" t="s">
+      <c r="C95" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="D95" s="16" t="s">
         <v>285</v>
+      </c>
+      <c r="E95" s="17" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,17 +2931,17 @@
         <f aca="false">CONCATENATE($B$2,":",B96)</f>
         <v>rico:RecordState</v>
       </c>
-      <c r="B96" s="15" t="s">
-        <v>286</v>
-      </c>
-      <c r="C96" s="15" t="s">
+      <c r="B96" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="D96" s="15" t="s">
+      <c r="C96" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="E96" s="16" t="s">
+      <c r="D96" s="16" t="s">
         <v>289</v>
+      </c>
+      <c r="E96" s="17" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2940,17 +2949,17 @@
         <f aca="false">CONCATENATE($B$2,":",B97)</f>
         <v>rico:Relation</v>
       </c>
-      <c r="B97" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="E97" s="16" t="s">
+      <c r="B97" s="16" t="s">
         <v>291</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="E97" s="17" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2958,15 +2967,15 @@
         <f aca="false">CONCATENATE($B$2,":",B98)</f>
         <v>rico:RepresentationType</v>
       </c>
-      <c r="B98" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="C98" s="15" t="s">
+      <c r="B98" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="D98" s="15"/>
-      <c r="E98" s="16" t="s">
+      <c r="C98" s="16" t="s">
         <v>294</v>
+      </c>
+      <c r="D98" s="16"/>
+      <c r="E98" s="17" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,15 +2983,15 @@
         <f aca="false">CONCATENATE($B$2,":",B99)</f>
         <v>rico:RoleType</v>
       </c>
-      <c r="B99" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="C99" s="15" t="s">
+      <c r="B99" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="D99" s="15"/>
-      <c r="E99" s="16" t="s">
+      <c r="C99" s="16" t="s">
         <v>297</v>
+      </c>
+      <c r="D99" s="16"/>
+      <c r="E99" s="17" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2990,17 +2999,17 @@
         <f aca="false">CONCATENATE($B$2,":",B100)</f>
         <v>rico:Rule</v>
       </c>
-      <c r="B100" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="D100" s="15" t="s">
+      <c r="B100" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="E100" s="16" t="s">
+      <c r="C100" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D100" s="16" t="s">
         <v>300</v>
+      </c>
+      <c r="E100" s="17" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,15 +3017,15 @@
         <f aca="false">CONCATENATE($B$2,":",B101)</f>
         <v>rico:RuleRelation</v>
       </c>
-      <c r="B101" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="C101" s="15" t="s">
+      <c r="B101" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="D101" s="15"/>
-      <c r="E101" s="16" t="s">
+      <c r="C101" s="16" t="s">
         <v>303</v>
+      </c>
+      <c r="D101" s="16"/>
+      <c r="E101" s="17" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3024,17 +3033,17 @@
         <f aca="false">CONCATENATE($B$2,":",B102)</f>
         <v>rico:RuleType</v>
       </c>
-      <c r="B102" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="C102" s="15" t="s">
+      <c r="B102" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="D102" s="15" t="s">
+      <c r="C102" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="D102" s="16" t="s">
         <v>307</v>
+      </c>
+      <c r="E102" s="17" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3042,15 +3051,15 @@
         <f aca="false">CONCATENATE($B$2,":",B103)</f>
         <v>rico:SequentialRelation</v>
       </c>
-      <c r="B103" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="C103" s="15" t="s">
+      <c r="B103" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="D103" s="15"/>
-      <c r="E103" s="16" t="s">
+      <c r="C103" s="16" t="s">
         <v>310</v>
+      </c>
+      <c r="D103" s="16"/>
+      <c r="E103" s="17" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,15 +3067,15 @@
         <f aca="false">CONCATENATE($B$2,":",B104)</f>
         <v>rico:SiblingRelation</v>
       </c>
-      <c r="B104" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="C104" s="15" t="s">
+      <c r="B104" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="D104" s="15"/>
-      <c r="E104" s="16" t="s">
+      <c r="C104" s="16" t="s">
         <v>313</v>
+      </c>
+      <c r="D104" s="16"/>
+      <c r="E104" s="17" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3074,17 +3083,17 @@
         <f aca="false">CONCATENATE($B$2,":",B105)</f>
         <v>rico:SingleDate</v>
       </c>
-      <c r="B105" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="C105" s="15" t="s">
+      <c r="B105" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="D105" s="15" t="s">
+      <c r="C105" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="E105" s="16" t="s">
+      <c r="D105" s="16" t="s">
         <v>317</v>
+      </c>
+      <c r="E105" s="17" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,15 +3101,15 @@
         <f aca="false">CONCATENATE($B$2,":",B106)</f>
         <v>rico:SpouseRelation</v>
       </c>
-      <c r="B106" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="C106" s="15" t="s">
+      <c r="B106" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="D106" s="15"/>
-      <c r="E106" s="16" t="s">
+      <c r="C106" s="16" t="s">
         <v>320</v>
+      </c>
+      <c r="D106" s="16"/>
+      <c r="E106" s="17" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3108,15 +3117,15 @@
         <f aca="false">CONCATENATE($B$2,":",B107)</f>
         <v>rico:TeachingRelation</v>
       </c>
-      <c r="B107" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="C107" s="15" t="s">
+      <c r="B107" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="D107" s="15"/>
-      <c r="E107" s="16" t="s">
+      <c r="C107" s="16" t="s">
         <v>323</v>
+      </c>
+      <c r="D107" s="16"/>
+      <c r="E107" s="17" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3124,15 +3133,15 @@
         <f aca="false">CONCATENATE($B$2,":",B108)</f>
         <v>rico:TemporalRelation</v>
       </c>
-      <c r="B108" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="C108" s="15" t="s">
+      <c r="B108" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="D108" s="15"/>
-      <c r="E108" s="16" t="s">
+      <c r="C108" s="16" t="s">
         <v>326</v>
+      </c>
+      <c r="D108" s="16"/>
+      <c r="E108" s="17" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3140,17 +3149,17 @@
         <f aca="false">CONCATENATE($B$2,":",B109)</f>
         <v>rico:Thing</v>
       </c>
-      <c r="B109" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="D109" s="15" t="s">
+      <c r="B109" s="16" t="s">
         <v>328</v>
       </c>
-      <c r="E109" s="16" t="s">
+      <c r="C109" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="D109" s="16" t="s">
         <v>329</v>
+      </c>
+      <c r="E109" s="17" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3158,17 +3167,17 @@
         <f aca="false">CONCATENATE($B$2,":",B110)</f>
         <v>rico:Title</v>
       </c>
-      <c r="B110" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="D110" s="15" t="s">
+      <c r="B110" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="E110" s="16" t="s">
+      <c r="C110" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="D110" s="16" t="s">
         <v>332</v>
+      </c>
+      <c r="E110" s="17" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3176,17 +3185,17 @@
         <f aca="false">CONCATENATE($B$2,":",B111)</f>
         <v>rico:Type</v>
       </c>
-      <c r="B111" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="D111" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="E111" s="16" t="s">
+      <c r="B111" s="16" t="s">
         <v>334</v>
+      </c>
+      <c r="C111" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="E111" s="17" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3194,15 +3203,15 @@
         <f aca="false">CONCATENATE($B$2,":",B112)</f>
         <v>rico:TypeRelation</v>
       </c>
-      <c r="B112" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="C112" s="15" t="s">
+      <c r="B112" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="D112" s="15"/>
-      <c r="E112" s="16" t="s">
+      <c r="C112" s="16" t="s">
         <v>337</v>
+      </c>
+      <c r="D112" s="16"/>
+      <c r="E112" s="17" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3210,17 +3219,17 @@
         <f aca="false">CONCATENATE($B$2,":",B113)</f>
         <v>rico:UnitOfMeasurement</v>
       </c>
-      <c r="B113" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="C113" s="15" t="s">
+      <c r="B113" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="D113" s="15" t="s">
+      <c r="C113" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="E113" s="16" t="s">
+      <c r="D113" s="16" t="s">
         <v>341</v>
+      </c>
+      <c r="E113" s="17" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,15 +3237,15 @@
         <f aca="false">CONCATENATE($B$2,":",B114)</f>
         <v>rico:WholePartRelation</v>
       </c>
-      <c r="B114" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="C114" s="15" t="s">
+      <c r="B114" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="D114" s="15"/>
-      <c r="E114" s="16" t="s">
+      <c r="C114" s="16" t="s">
         <v>344</v>
+      </c>
+      <c r="D114" s="16"/>
+      <c r="E114" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,15 +3253,15 @@
         <f aca="false">CONCATENATE($B$2,":",B115)</f>
         <v>rico:WorkRelation</v>
       </c>
-      <c r="B115" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="C115" s="15" t="s">
+      <c r="B115" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="D115" s="15"/>
-      <c r="E115" s="16" t="s">
+      <c r="C115" s="16" t="s">
         <v>347</v>
+      </c>
+      <c r="D115" s="16"/>
+      <c r="E115" s="17" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>